<commit_message>
new file:   Cage No108.csv 	new file:   Cage No65.csv 	new file:   Cage No78.csv 	modified:   Storage.xlsx 	modified:   Summary.xlsx 	modified:   Test.xlsx
</commit_message>
<xml_diff>
--- a/Storage.xlsx
+++ b/Storage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRIMBLE\Desktop\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1E9059-3B43-4619-8D6D-D44EF0F28B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA519DE7-C421-4567-BB59-39EAF4810796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0CCE4925-3B03-476B-B7CB-6475AF2C4D51}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="22">
   <si>
     <t>A</t>
   </si>
@@ -1958,10 +1958,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE54B524-2C50-4E6A-B5CD-C3B977ECFC66}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2007,26 +2007,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>296001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" location="Title!A1" display="Click here to return" xr:uid="{9C51AD95-256B-426E-916B-D0B0FE6A573F}"/>

</xml_diff>

<commit_message>
modified:   Storage.xlsx 	new file:   Summary.xlsx 	modified:   Test.xlsx
</commit_message>
<xml_diff>
--- a/Storage.xlsx
+++ b/Storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRIMBLE\Desktop\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05688058-194E-4BD8-A86F-4E1276BB6EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CE39CF-49BD-4299-9E59-62D0E695D9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="8964" firstSheet="26" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="8964" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="13">
   <si>
     <t>Cage No.</t>
   </si>
@@ -152,33 +152,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>PITT</t>
-  </si>
-  <si>
-    <t>GRD</t>
-  </si>
-  <si>
-    <t>T-RAD-B</t>
-  </si>
-  <si>
-    <t>HTH</t>
-  </si>
-  <si>
-    <t>Sheet-2</t>
-  </si>
-  <si>
-    <t>211/1</t>
-  </si>
-  <si>
-    <t>RND Spigot</t>
-  </si>
-  <si>
-    <t>TDFL STRT</t>
-  </si>
-  <si>
-    <t>T-Taper</t>
   </si>
 </sst>
 </file>
@@ -611,7 +584,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +609,7 @@
       </c>
       <c r="B2" s="10">
         <f>'1-A-R'!$D$1</f>
-        <v>776</v>
+        <v>0</v>
       </c>
       <c r="C2" s="10">
         <f>'1-B-R'!$D$1</f>
@@ -701,15 +674,15 @@
       </c>
       <c r="B5" s="10">
         <f>'4-A-R'!$D$1</f>
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="C5" s="10">
         <f>'4-B-R'!$D$1</f>
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="D5" s="10">
         <f>'4-C-R'!$D$1</f>
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -1274,10 +1247,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,48 +1269,28 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>967001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1352,10 +1305,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,71 +1327,28 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
-        <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>296001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>296001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>211</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1453,10 +1363,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,51 +1385,28 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
-        <v>108</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>296001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3">
-        <v>223</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +1772,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1904,9 +1791,6 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
-        <v>776</v>
-      </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2757,7 +2641,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>